<commit_message>
Add comprehensive Lightsail deployment guide and update Excel template
</commit_message>
<xml_diff>
--- a/RX_Combined_MR_Doctor_Template.xlsx
+++ b/RX_Combined_MR_Doctor_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudhanshu Pandey\Desktop\Rx Tool Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB798E7-0F5D-4529-974D-D14248529C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCA56F-C5A1-4CAE-B253-DE201D1CE90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{92668EB0-D0A4-4082-B7FC-C4F4472D29B5}"/>
   </bookViews>
@@ -3821,8 +3821,8 @@
   <dimension ref="A1:E961"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A259" sqref="A259:XFD259"/>
+      <pane ySplit="1" topLeftCell="A602" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A618" sqref="A618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14325,7 +14325,7 @@
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A618" s="7">
-        <v>3533139</v>
+        <v>3695822</v>
       </c>
       <c r="B618" s="19" t="s">
         <v>618</v>
@@ -20179,6 +20179,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A863A87AF39A7645A4E913E83E3BB7D7" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab37ef2b87aa09264eeeb6d2ebf6aff0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1fcc10ef-7790-4427-9d79-66d9aeb28622" xmlns:ns4="0c2a2d46-e6cf-4e8e-a681-61d31a2adbfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="959a8d1e19b8fdc59318050feea1bf42" ns3:_="" ns4:_="">
     <xsd:import namespace="1fcc10ef-7790-4427-9d79-66d9aeb28622"/>
@@ -20405,15 +20414,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -20423,6 +20423,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E196EB43-6810-45C4-9606-9015870D7B17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE670ECF-0179-4F88-B302-A3886BF94B3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20437,14 +20445,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E196EB43-6810-45C4-9606-9015870D7B17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>